<commit_message>
add two questions and update choices for crops and subsectors
</commit_message>
<xml_diff>
--- a/app/config/tables/business/forms/business/business.xlsx
+++ b/app/config/tables/business/forms/business/business.xlsx
@@ -20,12 +20,12 @@
     <sheet name="model" sheetId="6" r:id="rId6"/>
     <sheet name="prompt_types" sheetId="9" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="227">
   <si>
     <t>comments</t>
   </si>
@@ -396,174 +396,24 @@
     <t>Choose the subsector of the business</t>
   </si>
   <si>
-    <t>maize</t>
-  </si>
-  <si>
-    <t>mahindi</t>
-  </si>
-  <si>
-    <t>beans</t>
-  </si>
-  <si>
-    <t>maharage</t>
-  </si>
-  <si>
-    <t>field peas</t>
-  </si>
-  <si>
-    <t>mikunde</t>
-  </si>
-  <si>
-    <t>cow peas</t>
-  </si>
-  <si>
-    <t>njegere</t>
-  </si>
-  <si>
-    <t>green gram</t>
-  </si>
-  <si>
-    <t>choroko</t>
-  </si>
-  <si>
-    <t>groundnuts</t>
-  </si>
-  <si>
-    <t>karanga</t>
-  </si>
-  <si>
-    <t>sunflower</t>
-  </si>
-  <si>
-    <t>alizeti</t>
-  </si>
-  <si>
-    <t>sesame</t>
-  </si>
-  <si>
-    <t>ufuta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">grapes </t>
-  </si>
-  <si>
-    <t>zabibu</t>
-  </si>
-  <si>
-    <t>greens</t>
-  </si>
-  <si>
-    <t>mboga za majani</t>
-  </si>
-  <si>
-    <t>fruits</t>
-  </si>
-  <si>
-    <t>matunda</t>
-  </si>
-  <si>
-    <t>vegetables</t>
-  </si>
-  <si>
-    <t xml:space="preserve">viungo </t>
-  </si>
-  <si>
-    <t>cereals/legumes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nafaka </t>
-  </si>
-  <si>
-    <t>cash crops</t>
-  </si>
-  <si>
-    <t>mazao ya biashara</t>
-  </si>
-  <si>
-    <t>banana</t>
-  </si>
-  <si>
-    <t>ndizi</t>
-  </si>
-  <si>
-    <t>sugarcane</t>
-  </si>
-  <si>
-    <t>miwa</t>
-  </si>
-  <si>
     <t>Other crop</t>
   </si>
   <si>
-    <t>mazao nyingine</t>
-  </si>
-  <si>
-    <t>cow</t>
-  </si>
-  <si>
     <t>Ngo'mbe</t>
   </si>
   <si>
-    <t>donkey</t>
-  </si>
-  <si>
     <t>Punda</t>
   </si>
   <si>
-    <t>goat</t>
-  </si>
-  <si>
-    <t>mbuzi</t>
-  </si>
-  <si>
-    <t>sheep</t>
-  </si>
-  <si>
-    <t>kondoo</t>
-  </si>
-  <si>
-    <t>pig</t>
-  </si>
-  <si>
-    <t>nguruwe</t>
-  </si>
-  <si>
-    <t>fowl</t>
-  </si>
-  <si>
     <t>Ndege (Kuku/Bata)</t>
   </si>
   <si>
-    <t>rabbits</t>
-  </si>
-  <si>
-    <t>sungura</t>
-  </si>
-  <si>
-    <t>milk</t>
-  </si>
-  <si>
-    <t>maziwa</t>
-  </si>
-  <si>
-    <t>eggs</t>
-  </si>
-  <si>
-    <t>mayai</t>
-  </si>
-  <si>
-    <t>butchered meat</t>
-  </si>
-  <si>
     <t>Nyama iliyochinjwa</t>
   </si>
   <si>
     <t>Other livestock</t>
   </si>
   <si>
-    <t>mifugo nyingine</t>
-  </si>
-  <si>
     <t>display.title.text.sw</t>
   </si>
   <si>
@@ -628,9 +478,6 @@
   </si>
   <si>
     <t>"subsector.csv"</t>
-  </si>
-  <si>
-    <t>(data('sector_type') === 1 || data('sector_type') === 2)</t>
   </si>
   <si>
     <t>choice_item.sector_number == data('sector_type')</t>
@@ -701,6 +548,168 @@
   </si>
   <si>
     <t>Sina uhakika</t>
+  </si>
+  <si>
+    <t>Maize</t>
+  </si>
+  <si>
+    <t>Mahindi</t>
+  </si>
+  <si>
+    <t>Beans/legumes</t>
+  </si>
+  <si>
+    <t>Jamii maharage</t>
+  </si>
+  <si>
+    <t>Groundnuts</t>
+  </si>
+  <si>
+    <t>Karanga</t>
+  </si>
+  <si>
+    <t>Sunflower</t>
+  </si>
+  <si>
+    <t>Alizeti</t>
+  </si>
+  <si>
+    <t>Sesame</t>
+  </si>
+  <si>
+    <t>Ufuta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grapes </t>
+  </si>
+  <si>
+    <t>Zabibu</t>
+  </si>
+  <si>
+    <t>Fruits</t>
+  </si>
+  <si>
+    <t>Matunda</t>
+  </si>
+  <si>
+    <t>Vegetables</t>
+  </si>
+  <si>
+    <t>Viungo au mboga</t>
+  </si>
+  <si>
+    <t>Cereals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nafaka </t>
+  </si>
+  <si>
+    <t>Banana</t>
+  </si>
+  <si>
+    <t>Ndizi</t>
+  </si>
+  <si>
+    <t>Sugarcane</t>
+  </si>
+  <si>
+    <t>Miwa</t>
+  </si>
+  <si>
+    <t>Charcoal</t>
+  </si>
+  <si>
+    <t>Mkaa</t>
+  </si>
+  <si>
+    <t>Forestry</t>
+  </si>
+  <si>
+    <t>Mazao ya misitu</t>
+  </si>
+  <si>
+    <t>Mazao nyingine</t>
+  </si>
+  <si>
+    <t>Cow</t>
+  </si>
+  <si>
+    <t>Donkey</t>
+  </si>
+  <si>
+    <t>Goat</t>
+  </si>
+  <si>
+    <t>Mbuzi</t>
+  </si>
+  <si>
+    <t>Sheep</t>
+  </si>
+  <si>
+    <t>Kondoo</t>
+  </si>
+  <si>
+    <t>Pig</t>
+  </si>
+  <si>
+    <t>Nguruwe</t>
+  </si>
+  <si>
+    <t>Fowl</t>
+  </si>
+  <si>
+    <t>Milk</t>
+  </si>
+  <si>
+    <t>Maziwa</t>
+  </si>
+  <si>
+    <t>Eggs</t>
+  </si>
+  <si>
+    <t>Mayai</t>
+  </si>
+  <si>
+    <t>Butchered meat</t>
+  </si>
+  <si>
+    <t>Fish/aquaculture</t>
+  </si>
+  <si>
+    <t>Ufugaji wa samaki</t>
+  </si>
+  <si>
+    <t>Mifugo nyingine</t>
+  </si>
+  <si>
+    <t>consent</t>
+  </si>
+  <si>
+    <t>business_owner_name</t>
+  </si>
+  <si>
+    <t>yes_no</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Do you consent to participate?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is the business owners name? </t>
+  </si>
+  <si>
+    <t>(data('sector_type') === 1 || data('sector_type') === 2 || data('sector_type') === 5)</t>
   </si>
 </sst>
 </file>
@@ -1447,10 +1456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="12.45"/>
@@ -1493,7 +1502,7 @@
         <v>7</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>211</v>
+        <v>160</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>6</v>
@@ -1516,269 +1525,303 @@
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="1"/>
-      <c r="D2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E2" t="s">
-        <v>99</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>90</v>
+      <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>217</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>89</v>
+        <v>224</v>
       </c>
       <c r="H2" s="21" t="s">
-        <v>89</v>
+        <v>224</v>
       </c>
       <c r="I2" s="2"/>
-      <c r="M2" s="4"/>
-    </row>
-    <row r="3" spans="1:14" ht="15.9">
+      <c r="M2" s="18"/>
+    </row>
+    <row r="3" spans="1:14" ht="12" customHeight="1">
       <c r="A3" s="1"/>
       <c r="D3" t="s">
         <v>110</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>111</v>
+      <c r="E3" t="s">
+        <v>99</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="H3" s="23" t="s">
-        <v>206</v>
+        <v>89</v>
+      </c>
+      <c r="H3" s="21" t="s">
+        <v>89</v>
       </c>
       <c r="I3" s="2"/>
       <c r="M3" s="4"/>
     </row>
     <row r="4" spans="1:14" ht="15.9">
+      <c r="A4" s="1"/>
       <c r="D4" t="s">
         <v>110</v>
       </c>
-      <c r="E4" t="s">
-        <v>106</v>
-      </c>
-      <c r="F4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" t="s">
-        <v>49</v>
-      </c>
-      <c r="H4" s="24" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="13" customHeight="1">
+      <c r="E4" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="H4" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="M4" s="4"/>
+    </row>
+    <row r="5" spans="1:14" ht="15.9">
       <c r="D5" t="s">
         <v>110</v>
       </c>
       <c r="E5" t="s">
+        <v>106</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" s="24" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="13" customHeight="1">
+      <c r="D6" t="s">
+        <v>110</v>
+      </c>
+      <c r="E6" t="s">
         <v>116</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F6" t="s">
         <v>42</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G6" t="s">
         <v>50</v>
       </c>
-      <c r="H5" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="L5" s="9"/>
-    </row>
-    <row r="6" spans="1:14" ht="15.9">
-      <c r="D6" t="s">
+      <c r="H6" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="L6" s="9"/>
+    </row>
+    <row r="7" spans="1:14" ht="15.9">
+      <c r="D7" t="s">
         <v>23</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F7" t="s">
         <v>33</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G7" t="s">
         <v>47</v>
       </c>
-      <c r="H6" s="26" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="12" customHeight="1">
-      <c r="D7" t="s">
+      <c r="H7" s="26" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="15.9">
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" t="s">
+        <v>218</v>
+      </c>
+      <c r="G8" t="s">
+        <v>225</v>
+      </c>
+      <c r="H8" s="30" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="12" customHeight="1">
+      <c r="D9" t="s">
         <v>31</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E9" t="s">
         <v>45</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F9" t="s">
         <v>34</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G9" t="s">
         <v>48</v>
       </c>
-      <c r="H7" s="27" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" s="20" customFormat="1">
-      <c r="D8" s="20" t="s">
+      <c r="H9" s="27" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" s="20" customFormat="1">
+      <c r="D10" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="20" t="s">
-        <v>193</v>
-      </c>
-      <c r="F8" s="20" t="s">
+      <c r="E10" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="F10" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="G8" s="20" t="s">
+      <c r="G10" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="H8" s="28" t="s">
+      <c r="H10" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="L8" s="20" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" s="19" customFormat="1">
-      <c r="B9" s="19" t="s">
-        <v>192</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" s="19" customFormat="1">
-      <c r="D10" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>194</v>
-      </c>
-      <c r="F10" s="19" t="s">
-        <v>196</v>
-      </c>
-      <c r="G10" s="19" t="s">
-        <v>195</v>
-      </c>
-      <c r="H10" s="29" t="s">
-        <v>195</v>
+      <c r="L10" s="20" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:14" s="19" customFormat="1">
       <c r="B11" s="19" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="15.9">
-      <c r="D12" t="s">
+        <v>142</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="19" customFormat="1">
+      <c r="D12" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="H12" s="29" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="19" customFormat="1">
+      <c r="B13" s="19" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="15.9">
+      <c r="D14" t="s">
         <v>13</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E14" t="s">
         <v>83</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F14" t="s">
         <v>81</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G14" t="s">
         <v>82</v>
       </c>
-      <c r="H12" s="31" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="15.9">
-      <c r="D13" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" t="s">
-        <v>85</v>
-      </c>
-      <c r="G13" t="s">
-        <v>86</v>
-      </c>
-      <c r="H13" s="32" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14">
-      <c r="D14" t="s">
-        <v>23</v>
-      </c>
-      <c r="F14" t="s">
-        <v>84</v>
-      </c>
-      <c r="G14" t="s">
-        <v>197</v>
-      </c>
-      <c r="H14" t="s">
-        <v>197</v>
+      <c r="H14" s="31" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="15.9">
       <c r="D15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="F15" t="s">
-        <v>43</v>
+        <v>85</v>
       </c>
       <c r="G15" t="s">
-        <v>198</v>
-      </c>
-      <c r="H15" s="30" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="15" customHeight="1">
+        <v>86</v>
+      </c>
+      <c r="H15" s="32" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
       <c r="D16" t="s">
-        <v>110</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>117</v>
+        <v>23</v>
       </c>
       <c r="F16" t="s">
-        <v>44</v>
+        <v>84</v>
       </c>
       <c r="G16" t="s">
-        <v>51</v>
-      </c>
-      <c r="H16" s="33" t="s">
-        <v>214</v>
-      </c>
-      <c r="L16" s="9"/>
-    </row>
-    <row r="17" spans="4:8" ht="15.9">
-      <c r="D17" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="H16" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="17" spans="4:12" ht="15.9">
+      <c r="D17" t="s">
         <v>31</v>
       </c>
       <c r="E17" t="s">
         <v>65</v>
       </c>
       <c r="F17" t="s">
+        <v>43</v>
+      </c>
+      <c r="G17" t="s">
+        <v>148</v>
+      </c>
+      <c r="H17" s="30" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="18" spans="4:12" ht="15" customHeight="1">
+      <c r="D18" t="s">
+        <v>110</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="F18" t="s">
+        <v>44</v>
+      </c>
+      <c r="G18" t="s">
+        <v>51</v>
+      </c>
+      <c r="H18" s="33" t="s">
+        <v>163</v>
+      </c>
+      <c r="L18" s="9"/>
+    </row>
+    <row r="19" spans="4:12" ht="15.9">
+      <c r="D19" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" t="s">
+        <v>65</v>
+      </c>
+      <c r="F19" t="s">
         <v>46</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G19" t="s">
         <v>28</v>
       </c>
-      <c r="H17" s="35" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="18" spans="4:8" ht="31.75">
-      <c r="D18" t="s">
+      <c r="H19" s="35" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="20" spans="4:12" ht="31.75">
+      <c r="D20" t="s">
         <v>23</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F20" t="s">
         <v>113</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G20" t="s">
         <v>115</v>
       </c>
-      <c r="H18" s="36" t="s">
-        <v>214</v>
+      <c r="H20" s="36" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -1792,7 +1835,7 @@
   <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D19" sqref="D18:D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="12.45"/>
@@ -1815,7 +1858,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>179</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="18" customHeight="1">
@@ -1826,10 +1869,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>180</v>
+        <v>130</v>
       </c>
       <c r="D2" t="s">
-        <v>181</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" customHeight="1">
@@ -1843,7 +1886,7 @@
         <v>67</v>
       </c>
       <c r="D3" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17.05" customHeight="1">
@@ -1857,7 +1900,7 @@
         <v>68</v>
       </c>
       <c r="D4" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17.05" customHeight="1">
@@ -1871,7 +1914,7 @@
         <v>69</v>
       </c>
       <c r="D5" t="s">
-        <v>184</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17.05" customHeight="1">
@@ -1882,10 +1925,10 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>185</v>
+        <v>135</v>
       </c>
       <c r="D6" t="s">
-        <v>186</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17.05" customHeight="1">
@@ -1896,10 +1939,10 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>187</v>
+        <v>137</v>
       </c>
       <c r="D7" t="s">
-        <v>188</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17.05" customHeight="1">
@@ -1910,10 +1953,10 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>189</v>
+        <v>139</v>
       </c>
       <c r="D8" t="s">
-        <v>190</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17.05" customHeight="1">
@@ -1927,7 +1970,7 @@
         <v>70</v>
       </c>
       <c r="D9" t="s">
-        <v>191</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16" customHeight="1">
@@ -1941,7 +1984,7 @@
         <v>30</v>
       </c>
       <c r="D11" s="37" t="s">
-        <v>222</v>
+        <v>171</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17.05" customHeight="1">
@@ -1955,7 +1998,7 @@
         <v>29</v>
       </c>
       <c r="D12" s="39" t="s">
-        <v>221</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="19" customHeight="1">
@@ -1969,7 +2012,7 @@
         <v>66</v>
       </c>
       <c r="D13" s="38" t="s">
-        <v>223</v>
+        <v>172</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="19" customHeight="1"/>
@@ -1983,8 +2026,8 @@
       <c r="C15" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="36" t="s">
-        <v>219</v>
+      <c r="D15" s="39" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.9">
@@ -1997,457 +2040,440 @@
       <c r="C16" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="36" t="s">
+      <c r="D16" s="39" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="19" customHeight="1"/>
+    <row r="18" spans="1:4" ht="15" customHeight="1">
+      <c r="A18" t="s">
+        <v>219</v>
+      </c>
+      <c r="B18" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="12" t="s">
+      <c r="C18" t="s">
+        <v>221</v>
+      </c>
+      <c r="D18" s="36"/>
+    </row>
+    <row r="19" spans="1:4" ht="15.9">
+      <c r="A19" t="s">
+        <v>219</v>
+      </c>
+      <c r="B19" t="s">
+        <v>222</v>
+      </c>
+      <c r="C19" t="s">
+        <v>223</v>
+      </c>
+      <c r="D19" s="36"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="B19" s="34" t="s">
+      <c r="B22" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="C19" s="34" t="s">
+      <c r="C22" s="34" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="12" t="s">
+    <row r="23" spans="1:4">
+      <c r="A23" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="B20" s="34" t="s">
+      <c r="B23" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="C20" s="34" t="s">
+      <c r="C23" s="34" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="12" t="s">
+    <row r="24" spans="1:4">
+      <c r="A24" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="B21" s="34" t="s">
+      <c r="B24" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="C21" s="34" t="s">
+      <c r="C24" s="34" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="6" t="s">
+    <row r="25" spans="1:4">
+      <c r="A25" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="6"/>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" t="s">
-        <v>194</v>
-      </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25" t="s">
-        <v>123</v>
-      </c>
-      <c r="D25" t="s">
-        <v>124</v>
+      <c r="B25" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" t="s">
-        <v>194</v>
-      </c>
-      <c r="B26">
-        <v>2</v>
-      </c>
-      <c r="C26" t="s">
-        <v>125</v>
-      </c>
-      <c r="D26" t="s">
-        <v>126</v>
-      </c>
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" t="s">
-        <v>194</v>
-      </c>
-      <c r="B27">
-        <v>3</v>
-      </c>
-      <c r="C27" t="s">
-        <v>127</v>
-      </c>
-      <c r="D27" t="s">
-        <v>128</v>
-      </c>
+      <c r="A27" s="6"/>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>194</v>
+        <v>144</v>
       </c>
       <c r="B28">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>129</v>
+        <v>173</v>
       </c>
       <c r="D28" t="s">
-        <v>130</v>
+        <v>174</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>194</v>
+        <v>144</v>
       </c>
       <c r="B29">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>131</v>
+        <v>175</v>
       </c>
       <c r="D29" t="s">
-        <v>132</v>
+        <v>176</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>194</v>
+        <v>144</v>
       </c>
       <c r="B30">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>133</v>
+        <v>177</v>
       </c>
       <c r="D30" t="s">
-        <v>134</v>
+        <v>178</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>194</v>
+        <v>144</v>
       </c>
       <c r="B31">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>135</v>
+        <v>179</v>
       </c>
       <c r="D31" t="s">
-        <v>136</v>
+        <v>180</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>194</v>
+        <v>144</v>
       </c>
       <c r="B32">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C32" t="s">
-        <v>137</v>
+        <v>181</v>
       </c>
       <c r="D32" t="s">
-        <v>138</v>
+        <v>182</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>194</v>
+        <v>144</v>
       </c>
       <c r="B33">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C33" t="s">
-        <v>139</v>
+        <v>183</v>
       </c>
       <c r="D33" t="s">
-        <v>140</v>
+        <v>184</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>194</v>
+        <v>144</v>
       </c>
       <c r="B34">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C34" t="s">
-        <v>141</v>
+        <v>185</v>
       </c>
       <c r="D34" t="s">
-        <v>142</v>
+        <v>186</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>194</v>
+        <v>144</v>
       </c>
       <c r="B35">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C35" t="s">
-        <v>143</v>
+        <v>187</v>
       </c>
       <c r="D35" t="s">
-        <v>144</v>
+        <v>188</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>194</v>
+        <v>144</v>
       </c>
       <c r="B36">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C36" t="s">
-        <v>145</v>
+        <v>189</v>
       </c>
       <c r="D36" t="s">
-        <v>146</v>
+        <v>190</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>194</v>
+        <v>144</v>
       </c>
       <c r="B37">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C37" t="s">
-        <v>147</v>
+        <v>191</v>
       </c>
       <c r="D37" t="s">
-        <v>148</v>
+        <v>192</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
+        <v>144</v>
+      </c>
+      <c r="B38">
+        <v>11</v>
+      </c>
+      <c r="C38" t="s">
+        <v>193</v>
+      </c>
+      <c r="D38" t="s">
         <v>194</v>
-      </c>
-      <c r="B38">
-        <v>14</v>
-      </c>
-      <c r="C38" t="s">
-        <v>149</v>
-      </c>
-      <c r="D38" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>194</v>
+        <v>144</v>
       </c>
       <c r="B39">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C39" t="s">
-        <v>151</v>
+        <v>195</v>
       </c>
       <c r="D39" t="s">
-        <v>152</v>
+        <v>196</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>194</v>
+        <v>144</v>
       </c>
       <c r="B40">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C40" t="s">
-        <v>153</v>
+        <v>197</v>
       </c>
       <c r="D40" t="s">
-        <v>154</v>
+        <v>198</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>194</v>
+        <v>144</v>
       </c>
       <c r="B41">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C41" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="D41" t="s">
-        <v>156</v>
+        <v>199</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>194</v>
+        <v>144</v>
       </c>
       <c r="B42">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C42" t="s">
-        <v>157</v>
+        <v>200</v>
       </c>
       <c r="D42" t="s">
-        <v>158</v>
+        <v>124</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>194</v>
+        <v>144</v>
       </c>
       <c r="B43">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C43" t="s">
-        <v>159</v>
+        <v>201</v>
       </c>
       <c r="D43" t="s">
-        <v>160</v>
+        <v>125</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>194</v>
+        <v>144</v>
       </c>
       <c r="B44">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C44" t="s">
-        <v>161</v>
+        <v>202</v>
       </c>
       <c r="D44" t="s">
-        <v>162</v>
+        <v>203</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>194</v>
+        <v>144</v>
       </c>
       <c r="B45">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C45" t="s">
-        <v>163</v>
+        <v>204</v>
       </c>
       <c r="D45" t="s">
-        <v>164</v>
+        <v>205</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>194</v>
+        <v>144</v>
       </c>
       <c r="B46">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C46" t="s">
-        <v>165</v>
+        <v>206</v>
       </c>
       <c r="D46" t="s">
-        <v>166</v>
+        <v>207</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>194</v>
+        <v>144</v>
       </c>
       <c r="B47">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C47" t="s">
-        <v>167</v>
+        <v>208</v>
       </c>
       <c r="D47" t="s">
-        <v>168</v>
+        <v>126</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>194</v>
+        <v>144</v>
       </c>
       <c r="B48">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C48" t="s">
-        <v>169</v>
+        <v>209</v>
       </c>
       <c r="D48" t="s">
-        <v>170</v>
+        <v>210</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>194</v>
+        <v>144</v>
       </c>
       <c r="B49">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C49" t="s">
-        <v>171</v>
+        <v>211</v>
       </c>
       <c r="D49" t="s">
-        <v>172</v>
+        <v>212</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>194</v>
+        <v>144</v>
       </c>
       <c r="B50">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C50" t="s">
-        <v>173</v>
+        <v>213</v>
       </c>
       <c r="D50" t="s">
-        <v>174</v>
+        <v>127</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>194</v>
+        <v>144</v>
       </c>
       <c r="B51">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C51" t="s">
-        <v>175</v>
+        <v>214</v>
       </c>
       <c r="D51" t="s">
-        <v>176</v>
+        <v>215</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>194</v>
+        <v>144</v>
       </c>
       <c r="B52">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C52" t="s">
-        <v>177</v>
+        <v>128</v>
       </c>
       <c r="D52" t="s">
-        <v>178</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -2734,16 +2760,16 @@
     </row>
     <row r="8" spans="1:12" ht="84.9" customHeight="1">
       <c r="A8" t="s">
-        <v>193</v>
+        <v>143</v>
       </c>
       <c r="B8" t="s">
         <v>62</v>
       </c>
       <c r="C8" t="s">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>203</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -2785,7 +2811,7 @@
         <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>179</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16.75" customHeight="1">
@@ -2796,10 +2822,10 @@
         <v>24</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>204</v>
+        <v>153</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>205</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16.75" customHeight="1">
@@ -2842,10 +2868,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="12.45"/>
@@ -2864,22 +2890,19 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" t="s">
+      <c r="A2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="B2" s="7" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -2889,34 +2912,37 @@
       <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="6"/>
+      <c r="B4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -2924,7 +2950,7 @@
         <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>121</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -2932,55 +2958,55 @@
         <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>196</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>79</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>218</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>80</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -2988,7 +3014,7 @@
         <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -2996,7 +3022,7 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -3004,48 +3030,64 @@
         <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>85</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
-      </c>
-      <c r="G21" s="6"/>
+        <v>84</v>
+      </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>31</v>
       </c>
       <c r="B22" t="s">
-        <v>46</v>
-      </c>
-      <c r="F22" s="6"/>
+        <v>43</v>
+      </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" t="s">
+        <v>44</v>
+      </c>
+      <c r="G23" s="6"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" t="s">
+        <v>46</v>
+      </c>
+      <c r="F24" s="6"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B25" t="s">
         <v>113</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Make authorization veo a text field for now and ensure user_id is passed through for verification and authorization
</commit_message>
<xml_diff>
--- a/app/config/tables/business/forms/business/business.xlsx
+++ b/app/config/tables/business/forms/business/business.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4100" yWindow="260" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="4100" yWindow="260" windowWidth="32220" windowHeight="16060" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="329">
   <si>
     <t>comments</t>
   </si>
@@ -1830,8 +1830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q49"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView topLeftCell="A28" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2656,11 +2656,9 @@
     </row>
     <row r="44" spans="2:12" ht="15" customHeight="1">
       <c r="D44" t="s">
-        <v>166</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>108</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="E44" s="6"/>
       <c r="F44" t="s">
         <v>41</v>
       </c>
@@ -3890,7 +3888,7 @@
   <dimension ref="A1:XFD33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -4104,7 +4102,7 @@
     </row>
     <row r="25" spans="1:16384">
       <c r="A25" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
Changed names of auth/ver fields to more clear and updated choices accordingly
</commit_message>
<xml_diff>
--- a/app/config/tables/business/forms/business/business.xlsx
+++ b/app/config/tables/business/forms/business/business.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4100" yWindow="260" windowWidth="32220" windowHeight="16060" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="4100" yWindow="260" windowWidth="32220" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -111,15 +111,6 @@
     <t>Business</t>
   </si>
   <si>
-    <t>Has the VEO authorized this business?</t>
-  </si>
-  <si>
-    <t>True</t>
-  </si>
-  <si>
-    <t>False</t>
-  </si>
-  <si>
     <t>select_one_integer</t>
   </si>
   <si>
@@ -156,9 +147,6 @@
     <t>sector_type_list</t>
   </si>
   <si>
-    <t>has_been_authorized_by_veo</t>
-  </si>
-  <si>
     <t>Enter the name of the business.</t>
   </si>
   <si>
@@ -210,9 +198,6 @@
     <t>callback</t>
   </si>
   <si>
-    <t>true_false_unsure</t>
-  </si>
-  <si>
     <t>Unsure</t>
   </si>
   <si>
@@ -432,9 +417,6 @@
     <t>Enter the id of the coordinator who verified the business.</t>
   </si>
   <si>
-    <t>Has the coordinator verified this business?</t>
-  </si>
-  <si>
     <t>end if</t>
   </si>
   <si>
@@ -486,12 +468,6 @@
     <t>Mwanaume</t>
   </si>
   <si>
-    <t>Kweli</t>
-  </si>
-  <si>
-    <t>Sio kweli</t>
-  </si>
-  <si>
     <t>Sina uhakika</t>
   </si>
   <si>
@@ -790,9 +766,6 @@
   </si>
   <si>
     <t>sw:Enter the enrollment date</t>
-  </si>
-  <si>
-    <t>has_been_verified_by_coordinator</t>
   </si>
   <si>
     <t>male_female_no</t>
@@ -1016,6 +989,33 @@
   </si>
   <si>
     <t>Mifugo nyingine</t>
+  </si>
+  <si>
+    <t>has_been_authorized_by_veo_as</t>
+  </si>
+  <si>
+    <t>has_been_verified_by_coordinator_as</t>
+  </si>
+  <si>
+    <t>valid_invalid_unsure</t>
+  </si>
+  <si>
+    <t>Invalid</t>
+  </si>
+  <si>
+    <t>Sio halali</t>
+  </si>
+  <si>
+    <t>Valid</t>
+  </si>
+  <si>
+    <t>Halali</t>
+  </si>
+  <si>
+    <t>Coordinator verified this business as:</t>
+  </si>
+  <si>
+    <t>VEO authorized this business as:</t>
   </si>
 </sst>
 </file>
@@ -1149,7 +1149,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="87">
+  <cellStyleXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1211,6 +1211,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1336,7 +1344,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="87">
+  <cellStyles count="95">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -1380,6 +1388,10 @@
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1422,6 +1434,10 @@
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="60"/>
   </cellStyles>
@@ -1830,8 +1846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q49"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1874,7 +1890,7 @@
         <v>7</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>6</v>
@@ -1903,16 +1919,16 @@
         <v>13</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="H2" s="19" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -1922,10 +1938,10 @@
     <row r="3" spans="1:14" s="29" customFormat="1" ht="12" customHeight="1">
       <c r="A3" s="28"/>
       <c r="B3" s="3" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -1942,19 +1958,19 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="H4" s="19" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -1966,19 +1982,19 @@
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="H5" s="19" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
@@ -1989,19 +2005,19 @@
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H6" s="34" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
@@ -2011,19 +2027,19 @@
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>26</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H7" s="35" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
@@ -2037,16 +2053,16 @@
         <v>13</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="H8" s="34" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
@@ -2061,13 +2077,13 @@
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H9" s="35" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
@@ -2077,19 +2093,19 @@
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="30" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H10" s="35" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
@@ -2099,33 +2115,33 @@
       <c r="B11" s="30"/>
       <c r="C11" s="30"/>
       <c r="D11" s="30" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F11" s="30" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="G11" s="30" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="H11" s="31" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="I11" s="30"/>
       <c r="J11" s="30"/>
       <c r="K11" s="30"/>
       <c r="L11" s="32" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
     </row>
     <row r="12" spans="1:14" s="29" customFormat="1">
       <c r="B12" s="36" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C12" s="36" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="D12" s="36"/>
       <c r="E12" s="36"/>
@@ -2140,19 +2156,19 @@
       <c r="B13" s="36"/>
       <c r="C13" s="36"/>
       <c r="D13" s="36" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="E13" s="36" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="F13" s="36" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="G13" s="36" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="H13" s="21" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="I13" s="36"/>
       <c r="J13" s="36"/>
@@ -2160,10 +2176,10 @@
     </row>
     <row r="14" spans="1:14" s="29" customFormat="1">
       <c r="B14" s="36" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C14" s="36" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="D14" s="36"/>
       <c r="E14" s="36"/>
@@ -2182,13 +2198,13 @@
       </c>
       <c r="E15" s="36"/>
       <c r="F15" s="36" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="G15" s="36" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="H15" s="21" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="I15" s="36"/>
       <c r="J15" s="36"/>
@@ -2196,7 +2212,7 @@
     </row>
     <row r="16" spans="1:14" s="29" customFormat="1">
       <c r="B16" s="36" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C16" s="36"/>
       <c r="D16" s="36"/>
@@ -2210,7 +2226,7 @@
     </row>
     <row r="17" spans="1:17" s="29" customFormat="1">
       <c r="B17" s="36" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C17" s="36"/>
       <c r="D17" s="36"/>
@@ -2225,16 +2241,16 @@
     <row r="18" spans="1:17" s="30" customFormat="1" ht="13">
       <c r="A18" s="39"/>
       <c r="D18" s="30" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F18" s="30" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="G18" s="40" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="H18" s="41" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="N18" s="18"/>
       <c r="O18" s="32"/>
@@ -2249,13 +2265,13 @@
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="H19" s="34" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
@@ -2263,7 +2279,7 @@
     </row>
     <row r="20" spans="1:17">
       <c r="B20" s="30" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -2279,17 +2295,17 @@
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="H21" s="35" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
@@ -2299,17 +2315,17 @@
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="H22" s="31" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
@@ -2317,7 +2333,7 @@
     </row>
     <row r="23" spans="1:17">
       <c r="B23" s="3" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -2336,16 +2352,16 @@
         <v>13</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="H24" s="35" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
@@ -2355,17 +2371,17 @@
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G25" s="35" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="H25" s="34" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
@@ -2373,7 +2389,7 @@
     </row>
     <row r="26" spans="1:17">
       <c r="B26" s="3" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -2396,10 +2412,10 @@
         <v>25</v>
       </c>
       <c r="G27" s="37" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="H27" s="38" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="I27" s="37"/>
       <c r="J27" s="37"/>
@@ -2409,19 +2425,19 @@
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="H28" s="19" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
@@ -2429,7 +2445,7 @@
     </row>
     <row r="29" spans="1:17">
       <c r="B29" s="3" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -2443,7 +2459,7 @@
     </row>
     <row r="30" spans="1:17">
       <c r="B30" s="3" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -2462,16 +2478,16 @@
         <v>13</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="H31" s="19" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
@@ -2479,10 +2495,10 @@
     </row>
     <row r="32" spans="1:17">
       <c r="B32" s="3" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
@@ -2501,13 +2517,13 @@
       </c>
       <c r="E33" s="37"/>
       <c r="F33" s="37" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G33" s="37" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="H33" s="38" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="I33" s="37"/>
       <c r="J33" s="37"/>
@@ -2517,19 +2533,19 @@
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H34" s="35" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
@@ -2537,7 +2553,7 @@
     </row>
     <row r="35" spans="2:12">
       <c r="B35" s="3" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
@@ -2551,7 +2567,7 @@
     </row>
     <row r="36" spans="2:12">
       <c r="B36" s="3" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
@@ -2565,7 +2581,7 @@
     </row>
     <row r="37" spans="2:12">
       <c r="B37" s="3" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -2581,14 +2597,14 @@
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="3" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
@@ -2597,7 +2613,7 @@
     </row>
     <row r="39" spans="2:12">
       <c r="B39" s="3" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -2614,13 +2630,13 @@
         <v>23</v>
       </c>
       <c r="F41" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="G41" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="H41" s="23" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="42" spans="2:12">
@@ -2628,30 +2644,30 @@
         <v>23</v>
       </c>
       <c r="F42" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="G42" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="H42" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="43" spans="2:12" ht="15">
       <c r="D43" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E43" t="s">
-        <v>61</v>
+        <v>322</v>
       </c>
       <c r="F43" t="s">
-        <v>255</v>
+        <v>321</v>
       </c>
       <c r="G43" t="s">
-        <v>135</v>
+        <v>327</v>
       </c>
       <c r="H43" s="22" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="44" spans="2:12" ht="15" customHeight="1">
@@ -2660,31 +2676,31 @@
       </c>
       <c r="E44" s="6"/>
       <c r="F44" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G44" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="H44" s="24" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="L44" s="9"/>
     </row>
     <row r="45" spans="2:12" ht="15">
       <c r="D45" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E45" t="s">
-        <v>61</v>
+        <v>322</v>
       </c>
       <c r="F45" t="s">
-        <v>43</v>
+        <v>320</v>
       </c>
       <c r="G45" t="s">
-        <v>28</v>
+        <v>328</v>
       </c>
       <c r="H45" s="25" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="46" spans="2:12" ht="30">
@@ -2692,55 +2708,55 @@
         <v>23</v>
       </c>
       <c r="F46" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="G46" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="H46" s="26" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="47" spans="2:12">
       <c r="D47" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="G47" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="H47" s="19" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
     </row>
     <row r="48" spans="2:12">
       <c r="D48" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="G48" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="H48" s="19" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
     </row>
     <row r="49" spans="4:8">
       <c r="D49" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="G49" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="H49" s="19" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -2758,8 +2774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2782,695 +2798,695 @@
         <v>6</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="18" customHeight="1">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="C2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" customHeight="1">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" customHeight="1">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D4" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" customHeight="1">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D5" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17" customHeight="1">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="C6" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D6" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" customHeight="1">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="C7" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D7" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" customHeight="1">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="C8" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D8" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17" customHeight="1">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D9" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16" customHeight="1">
       <c r="A11" t="s">
-        <v>61</v>
+        <v>322</v>
       </c>
       <c r="B11" s="10">
         <v>0</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>30</v>
+        <v>323</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>154</v>
+        <v>324</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" customHeight="1">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>322</v>
       </c>
       <c r="B12" s="10">
         <v>1</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>29</v>
+        <v>325</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>153</v>
+        <v>326</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="19" customHeight="1">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>322</v>
       </c>
       <c r="B13">
         <v>-1</v>
       </c>
       <c r="C13" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="19" customHeight="1"/>
     <row r="15" spans="1:4" ht="15" customHeight="1">
       <c r="A15" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="B15" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="B16" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="B17" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="C17" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="19" customHeight="1"/>
     <row r="19" spans="1:4" ht="15" customHeight="1">
       <c r="A19" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="B19" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C19" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="B20" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="C20" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="12" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="12" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="12" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B25" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C25" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="D25" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B28" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="C28" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="D28" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B29" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="C29" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="D29" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B30" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="C30" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="D30" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B31" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="C31" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="D31" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B32" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="C32" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="D32" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B33" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="C33" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="D33" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B34" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="C34" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="D34" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B35" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="C35" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="D35" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B36" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="C36" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="D36" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B37" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="C37" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="D37" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B38" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="C38" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="D38" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B39" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="C39" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="D39" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B40" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="C40" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="D40" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B41" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="C41" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="D41" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B42" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="C42" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="D42" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B43" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="C43" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="D43" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B44" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="C44" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="D44" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B45" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="C45" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="D45" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B46" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="C46" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="D46" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B47" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="C47" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="D47" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B48" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="C48" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="D48" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B49" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="C49" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="D49" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B50" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="C50" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="D50" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B51" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="C51" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="D51" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B52" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="C52" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="D52" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="B56" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="C56" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="D56" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="B57" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="C57" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="D57" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="B58" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="C58" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D58" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
+        <v>232</v>
+      </c>
+      <c r="B59" t="s">
+        <v>236</v>
+      </c>
+      <c r="C59" t="s">
+        <v>236</v>
+      </c>
+      <c r="D59" t="s">
         <v>240</v>
-      </c>
-      <c r="B59" t="s">
-        <v>244</v>
-      </c>
-      <c r="C59" t="s">
-        <v>244</v>
-      </c>
-      <c r="D59" t="s">
-        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -3499,13 +3515,13 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -3516,19 +3532,19 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" t="s">
         <v>51</v>
-      </c>
-      <c r="B2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E2" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -3563,150 +3579,150 @@
   <sheetData>
     <row r="1" spans="1:11" ht="75">
       <c r="A1" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>60</v>
-      </c>
       <c r="E1" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="J1" t="s">
         <v>87</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>88</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="J1" t="s">
-        <v>92</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="F2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="I2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="J2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="K2" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>256</v>
+      </c>
+      <c r="I3" t="s">
         <v>94</v>
       </c>
-      <c r="B3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E3" t="s">
-        <v>96</v>
-      </c>
-      <c r="F3" t="s">
-        <v>96</v>
-      </c>
-      <c r="G3" s="18" t="s">
-        <v>264</v>
-      </c>
-      <c r="H3" s="18" t="s">
-        <v>265</v>
-      </c>
-      <c r="I3" t="s">
-        <v>99</v>
-      </c>
       <c r="J3" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="K3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B4" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G4" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="F4" t="s">
-        <v>96</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>101</v>
-      </c>
       <c r="H4" s="18" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="I4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="J4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="K4" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E5" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="F5" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="H5" s="18" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="I5" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="J5" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="K5" t="s">
         <v>26</v>
@@ -3714,74 +3730,74 @@
     </row>
     <row r="6" spans="1:11" ht="15">
       <c r="A6" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B6" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E6" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="F6" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="I6" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="J6" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="K6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15">
       <c r="A7" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B7" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E7" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="F7" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="I7" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="J7" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="K7" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="85" customHeight="1">
       <c r="A9" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C9" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -3823,7 +3839,7 @@
         <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16.75" customHeight="1">
@@ -3834,10 +3850,10 @@
         <v>24</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16.75" customHeight="1">
@@ -3869,7 +3885,7 @@
         <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -3887,8 +3903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -3911,15 +3927,15 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -3927,10 +3943,10 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -3938,7 +3954,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B5" t="s">
         <v>26</v>
@@ -3950,7 +3966,7 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G6" s="6"/>
     </row>
@@ -3959,31 +3975,31 @@
         <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="B9" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="B10" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -3991,7 +4007,7 @@
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -3999,23 +4015,23 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="B14" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -4023,15 +4039,15 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:16384">
@@ -4044,10 +4060,10 @@
     </row>
     <row r="18" spans="1:16384">
       <c r="A18" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="B18" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:16384">
@@ -4055,7 +4071,7 @@
         <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="20" spans="1:16384">
@@ -4063,15 +4079,15 @@
         <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:16384">
       <c r="A21" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="B21" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:16384">
@@ -4079,7 +4095,7 @@
         <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="G22" s="6"/>
     </row>
@@ -4088,16 +4104,16 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F23" s="6"/>
     </row>
     <row r="24" spans="1:16384">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>255</v>
+        <v>321</v>
       </c>
     </row>
     <row r="25" spans="1:16384">
@@ -4105,15 +4121,15 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:16384">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>320</v>
       </c>
     </row>
     <row r="27" spans="1:16384">
@@ -4121,31 +4137,31 @@
         <v>23</v>
       </c>
       <c r="B27" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:16384">
       <c r="A28" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="B28" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
     </row>
     <row r="29" spans="1:16384">
       <c r="A29" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="B29" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
     </row>
     <row r="30" spans="1:16384">
       <c r="A30" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="B30" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
     </row>
     <row r="31" spans="1:16384">
@@ -4153,7 +4169,7 @@
         <v>23</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -20540,10 +20556,10 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B33" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -20573,7 +20589,7 @@
   <sheetData>
     <row r="6" spans="1:2">
       <c r="A6" s="15" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>3</v>
@@ -20581,10 +20597,10 @@
     </row>
     <row r="7" spans="1:2" ht="13">
       <c r="A7" s="16" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update coordinator verification workflow and closeWindow where applicable
</commit_message>
<xml_diff>
--- a/app/config/tables/business/forms/business/business.xlsx
+++ b/app/config/tables/business/forms/business/business.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4100" yWindow="260" windowWidth="32220" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="4100" yWindow="260" windowWidth="32220" windowHeight="16060" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="320">
   <si>
     <t>comments</t>
   </si>
@@ -715,39 +715,6 @@
   </si>
   <si>
     <t xml:space="preserve">Thank you for your time.  </t>
-  </si>
-  <si>
-    <t>Choose the subvillage</t>
-  </si>
-  <si>
-    <t>sw:Choose the subvillage</t>
-  </si>
-  <si>
-    <t>subvillage_list</t>
-  </si>
-  <si>
-    <t>Subvillage12</t>
-  </si>
-  <si>
-    <t>Subvillage11</t>
-  </si>
-  <si>
-    <t>Subvillage31</t>
-  </si>
-  <si>
-    <t>Subvillage41</t>
-  </si>
-  <si>
-    <t>sw:Subvillage12</t>
-  </si>
-  <si>
-    <t>sw:Subvillage11</t>
-  </si>
-  <si>
-    <t>sw:Subvillage31</t>
-  </si>
-  <si>
-    <t>sw:Subvillage41</t>
   </si>
   <si>
     <t>Enter the authorization date</t>
@@ -1016,6 +983,12 @@
   </si>
   <si>
     <t>VEO authorized this business as:</t>
+  </si>
+  <si>
+    <t>Enter the subvillage</t>
+  </si>
+  <si>
+    <t>sw:Enter the subvillage</t>
   </si>
 </sst>
 </file>
@@ -1846,8 +1819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+    <sheetView topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1961,16 +1934,16 @@
         <v>158</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="H4" s="19" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -2050,19 +2023,17 @@
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>232</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
         <v>37</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="H8" s="34" t="s">
-        <v>231</v>
+        <v>319</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
@@ -2133,7 +2104,7 @@
       <c r="J11" s="30"/>
       <c r="K11" s="30"/>
       <c r="L11" s="32" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
     </row>
     <row r="12" spans="1:14" s="29" customFormat="1">
@@ -2244,13 +2215,13 @@
         <v>29</v>
       </c>
       <c r="F18" s="30" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="G18" s="40" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
       <c r="H18" s="41" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="N18" s="18"/>
       <c r="O18" s="32"/>
@@ -2352,7 +2323,7 @@
         <v>13</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>32</v>
@@ -2658,13 +2629,13 @@
         <v>28</v>
       </c>
       <c r="E43" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
       <c r="F43" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
       <c r="G43" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
       <c r="H43" s="22" t="s">
         <v>141</v>
@@ -2691,13 +2662,13 @@
         <v>28</v>
       </c>
       <c r="E45" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
       <c r="F45" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
       <c r="G45" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
       <c r="H45" s="25" t="s">
         <v>142</v>
@@ -2725,10 +2696,10 @@
         <v>166</v>
       </c>
       <c r="G47" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="H47" s="19" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
     </row>
     <row r="48" spans="2:12">
@@ -2739,10 +2710,10 @@
         <v>167</v>
       </c>
       <c r="G48" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="H48" s="19" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
     </row>
     <row r="49" spans="4:8">
@@ -2753,10 +2724,10 @@
         <v>168</v>
       </c>
       <c r="G49" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="H49" s="19" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -2772,10 +2743,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView topLeftCell="A35" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2915,35 +2886,35 @@
     </row>
     <row r="11" spans="1:4" ht="16" customHeight="1">
       <c r="A11" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
       <c r="B11" s="10">
         <v>0</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" customHeight="1">
       <c r="A12" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
       <c r="B12" s="10">
         <v>1</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="19" customHeight="1">
       <c r="A13" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
       <c r="B13">
         <v>-1</v>
@@ -2958,7 +2929,7 @@
     <row r="14" spans="1:4" ht="19" customHeight="1"/>
     <row r="15" spans="1:4" ht="15" customHeight="1">
       <c r="A15" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="B15" t="s">
         <v>68</v>
@@ -2972,7 +2943,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="B16" t="s">
         <v>69</v>
@@ -2986,16 +2957,16 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="B17" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="C17" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="19" customHeight="1"/>
@@ -3091,10 +3062,10 @@
         <v>179</v>
       </c>
       <c r="C28" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="D28" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -3102,13 +3073,13 @@
         <v>126</v>
       </c>
       <c r="B29" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="C29" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="D29" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -3119,10 +3090,10 @@
         <v>180</v>
       </c>
       <c r="C30" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="D30" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -3133,10 +3104,10 @@
         <v>181</v>
       </c>
       <c r="C31" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="D31" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -3147,10 +3118,10 @@
         <v>182</v>
       </c>
       <c r="C32" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
       <c r="D32" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -3158,13 +3129,13 @@
         <v>126</v>
       </c>
       <c r="B33" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="C33" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="D33" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -3175,10 +3146,10 @@
         <v>183</v>
       </c>
       <c r="C34" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="D34" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -3189,10 +3160,10 @@
         <v>184</v>
       </c>
       <c r="C35" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="D35" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -3200,13 +3171,13 @@
         <v>126</v>
       </c>
       <c r="B36" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="C36" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
       <c r="D36" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -3217,10 +3188,10 @@
         <v>185</v>
       </c>
       <c r="C37" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="D37" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -3231,10 +3202,10 @@
         <v>186</v>
       </c>
       <c r="C38" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="D38" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -3242,13 +3213,13 @@
         <v>126</v>
       </c>
       <c r="B39" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="C39" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="D39" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -3256,13 +3227,13 @@
         <v>126</v>
       </c>
       <c r="B40" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="C40" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="D40" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -3273,10 +3244,10 @@
         <v>161</v>
       </c>
       <c r="C41" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="D41" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -3287,7 +3258,7 @@
         <v>187</v>
       </c>
       <c r="C42" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
       <c r="D42" t="s">
         <v>107</v>
@@ -3301,7 +3272,7 @@
         <v>188</v>
       </c>
       <c r="C43" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="D43" t="s">
         <v>108</v>
@@ -3315,10 +3286,10 @@
         <v>189</v>
       </c>
       <c r="C44" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="D44" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -3329,10 +3300,10 @@
         <v>190</v>
       </c>
       <c r="C45" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="D45" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -3343,10 +3314,10 @@
         <v>191</v>
       </c>
       <c r="C46" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
       <c r="D46" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -3357,7 +3328,7 @@
         <v>192</v>
       </c>
       <c r="C47" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="D47" t="s">
         <v>109</v>
@@ -3371,10 +3342,10 @@
         <v>193</v>
       </c>
       <c r="C48" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
       <c r="D48" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -3385,10 +3356,10 @@
         <v>194</v>
       </c>
       <c r="C49" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="D49" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -3399,7 +3370,7 @@
         <v>195</v>
       </c>
       <c r="C50" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="D50" t="s">
         <v>110</v>
@@ -3410,13 +3381,13 @@
         <v>126</v>
       </c>
       <c r="B51" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="C51" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
       <c r="D51" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -3424,69 +3395,13 @@
         <v>126</v>
       </c>
       <c r="B52" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
       <c r="C52" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
       <c r="D52" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" t="s">
-        <v>232</v>
-      </c>
-      <c r="B56" t="s">
-        <v>233</v>
-      </c>
-      <c r="C56" t="s">
-        <v>233</v>
-      </c>
-      <c r="D56" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" t="s">
-        <v>232</v>
-      </c>
-      <c r="B57" t="s">
-        <v>234</v>
-      </c>
-      <c r="C57" t="s">
-        <v>234</v>
-      </c>
-      <c r="D57" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" t="s">
-        <v>232</v>
-      </c>
-      <c r="B58" t="s">
-        <v>235</v>
-      </c>
-      <c r="C58" t="s">
-        <v>235</v>
-      </c>
-      <c r="D58" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59" t="s">
-        <v>232</v>
-      </c>
-      <c r="B59" t="s">
-        <v>236</v>
-      </c>
-      <c r="C59" t="s">
-        <v>236</v>
-      </c>
-      <c r="D59" t="s">
-        <v>240</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -3561,8 +3476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -3614,7 +3529,7 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="B2" t="s">
         <v>90</v>
@@ -3638,7 +3553,7 @@
         <v>94</v>
       </c>
       <c r="K2" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -3655,10 +3570,10 @@
         <v>91</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="H3" s="18" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="I3" t="s">
         <v>94</v>
@@ -3713,10 +3628,10 @@
         <v>91</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="H5" s="18" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="I5" t="s">
         <v>94</v>
@@ -3742,10 +3657,10 @@
         <v>91</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="I6" t="s">
         <v>94</v>
@@ -3771,10 +3686,10 @@
         <v>91</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="I7" t="s">
         <v>94</v>
@@ -3797,7 +3712,7 @@
         <v>131</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -3903,8 +3818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -3963,7 +3878,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
         <v>37</v>
@@ -4113,7 +4028,7 @@
         <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
     </row>
     <row r="25" spans="1:16384">
@@ -4129,7 +4044,7 @@
         <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
     </row>
     <row r="27" spans="1:16384">
@@ -4169,7 +4084,7 @@
         <v>23</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -20559,7 +20474,7 @@
         <v>29</v>
       </c>
       <c r="B33" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix business form to allow editing of secondary phone number
</commit_message>
<xml_diff>
--- a/app/config/tables/business/forms/business/business.xlsx
+++ b/app/config/tables/business/forms/business/business.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="15800" yWindow="7460" windowWidth="21920" windowHeight="17140" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="15800" yWindow="7460" windowWidth="34000" windowHeight="21760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -645,9 +645,6 @@
     <t xml:space="preserve">if </t>
   </si>
   <si>
-    <t>selected('has_secondary_phone_number', 'yes')</t>
-  </si>
-  <si>
     <t>Enter the secondary phone number.</t>
   </si>
   <si>
@@ -1016,6 +1013,9 @@
   </si>
   <si>
     <t>Kiswahili</t>
+  </si>
+  <si>
+    <t>data('has_secondary_phone_number') === 'yes'</t>
   </si>
 </sst>
 </file>
@@ -1856,8 +1856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q49"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1938,7 +1938,7 @@
         <v>151</v>
       </c>
       <c r="H2" s="39" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -1971,16 +1971,16 @@
         <v>154</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>221</v>
-      </c>
       <c r="H4" s="39" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -2004,7 +2004,7 @@
         <v>79</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
@@ -2027,7 +2027,7 @@
         <v>78</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
@@ -2067,10 +2067,10 @@
         <v>36</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H8" s="37" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
@@ -2135,13 +2135,13 @@
         <v>105</v>
       </c>
       <c r="H11" s="38" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I11" s="27"/>
       <c r="J11" s="27"/>
       <c r="K11" s="27"/>
       <c r="L11" s="29" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="12" spans="1:14" s="26" customFormat="1">
@@ -2173,10 +2173,10 @@
         <v>126</v>
       </c>
       <c r="G13" s="41" t="s">
+        <v>311</v>
+      </c>
+      <c r="H13" s="41" t="s">
         <v>312</v>
-      </c>
-      <c r="H13" s="41" t="s">
-        <v>313</v>
       </c>
       <c r="I13" s="33"/>
       <c r="J13" s="33"/>
@@ -2212,7 +2212,7 @@
         <v>192</v>
       </c>
       <c r="H15" s="41" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="I15" s="33"/>
       <c r="J15" s="33"/>
@@ -2252,13 +2252,13 @@
         <v>28</v>
       </c>
       <c r="F18" s="27" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G18" s="42" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H18" s="42" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="N18" s="18"/>
       <c r="O18" s="29"/>
@@ -2279,7 +2279,7 @@
         <v>152</v>
       </c>
       <c r="H19" s="37" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
@@ -2333,7 +2333,7 @@
         <v>196</v>
       </c>
       <c r="H22" s="38" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
@@ -2360,7 +2360,7 @@
         <v>13</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>31</v>
@@ -2389,7 +2389,7 @@
         <v>200</v>
       </c>
       <c r="H25" s="37" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
@@ -2445,7 +2445,7 @@
         <v>203</v>
       </c>
       <c r="H28" s="39" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
@@ -2495,7 +2495,7 @@
         <v>204</v>
       </c>
       <c r="H31" s="39" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
@@ -2506,7 +2506,7 @@
         <v>205</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>206</v>
+        <v>328</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
@@ -2528,10 +2528,10 @@
         <v>35</v>
       </c>
       <c r="G33" s="34" t="s">
+        <v>206</v>
+      </c>
+      <c r="H33" s="35" t="s">
         <v>207</v>
-      </c>
-      <c r="H33" s="35" t="s">
-        <v>208</v>
       </c>
       <c r="I33" s="34"/>
       <c r="J33" s="34"/>
@@ -2589,7 +2589,7 @@
     </row>
     <row r="37" spans="2:12">
       <c r="B37" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -2605,17 +2605,17 @@
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="G38" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="G38" s="3" t="s">
-        <v>212</v>
-      </c>
       <c r="H38" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
@@ -2660,7 +2660,7 @@
         <v>127</v>
       </c>
       <c r="H42" s="19" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="43" spans="2:12" ht="15">
@@ -2668,16 +2668,16 @@
         <v>27</v>
       </c>
       <c r="E43" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F43" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G43" s="39" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H43" s="43" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="44" spans="2:12" ht="15" customHeight="1">
@@ -2701,16 +2701,16 @@
         <v>27</v>
       </c>
       <c r="E45" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F45" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G45" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H45" s="23" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="46" spans="2:12" ht="30">
@@ -2735,10 +2735,10 @@
         <v>162</v>
       </c>
       <c r="G47" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H47" s="39" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="48" spans="2:12">
@@ -2749,10 +2749,10 @@
         <v>163</v>
       </c>
       <c r="G48" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H48" s="39" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="49" spans="4:8">
@@ -2763,10 +2763,10 @@
         <v>164</v>
       </c>
       <c r="G49" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H49" s="39" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -2925,35 +2925,35 @@
     </row>
     <row r="11" spans="1:4" ht="16" customHeight="1">
       <c r="A11" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B11" s="10">
         <v>0</v>
       </c>
       <c r="C11" s="11" t="s">
+        <v>288</v>
+      </c>
+      <c r="D11" s="24" t="s">
         <v>289</v>
-      </c>
-      <c r="D11" s="24" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" customHeight="1">
       <c r="A12" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B12" s="10">
         <v>1</v>
       </c>
       <c r="C12" s="11" t="s">
+        <v>290</v>
+      </c>
+      <c r="D12" s="17" t="s">
         <v>291</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="19" customHeight="1">
       <c r="A13" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B13">
         <v>-1</v>
@@ -2968,7 +2968,7 @@
     <row r="14" spans="1:4" ht="19" customHeight="1"/>
     <row r="15" spans="1:4" ht="15" customHeight="1">
       <c r="A15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B15" t="s">
         <v>67</v>
@@ -2982,7 +2982,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B16" t="s">
         <v>68</v>
@@ -2996,16 +2996,16 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
+        <v>215</v>
+      </c>
+      <c r="B17" t="s">
         <v>216</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>217</v>
       </c>
-      <c r="C17" t="s">
-        <v>218</v>
-      </c>
       <c r="D17" s="39" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="19" customHeight="1"/>
@@ -3020,7 +3020,7 @@
         <v>148</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -3034,7 +3034,7 @@
         <v>150</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -3101,10 +3101,10 @@
         <v>173</v>
       </c>
       <c r="C28" t="s">
+        <v>230</v>
+      </c>
+      <c r="D28" t="s">
         <v>231</v>
-      </c>
-      <c r="D28" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -3112,13 +3112,13 @@
         <v>125</v>
       </c>
       <c r="B29" t="s">
+        <v>232</v>
+      </c>
+      <c r="C29" t="s">
         <v>233</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>234</v>
-      </c>
-      <c r="D29" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -3129,10 +3129,10 @@
         <v>174</v>
       </c>
       <c r="C30" t="s">
+        <v>235</v>
+      </c>
+      <c r="D30" t="s">
         <v>236</v>
-      </c>
-      <c r="D30" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -3143,10 +3143,10 @@
         <v>175</v>
       </c>
       <c r="C31" t="s">
+        <v>237</v>
+      </c>
+      <c r="D31" t="s">
         <v>238</v>
-      </c>
-      <c r="D31" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -3157,10 +3157,10 @@
         <v>176</v>
       </c>
       <c r="C32" t="s">
+        <v>239</v>
+      </c>
+      <c r="D32" t="s">
         <v>240</v>
-      </c>
-      <c r="D32" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -3168,13 +3168,13 @@
         <v>125</v>
       </c>
       <c r="B33" t="s">
+        <v>241</v>
+      </c>
+      <c r="C33" t="s">
         <v>242</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>243</v>
-      </c>
-      <c r="D33" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -3185,10 +3185,10 @@
         <v>177</v>
       </c>
       <c r="C34" t="s">
+        <v>244</v>
+      </c>
+      <c r="D34" t="s">
         <v>245</v>
-      </c>
-      <c r="D34" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -3199,10 +3199,10 @@
         <v>178</v>
       </c>
       <c r="C35" t="s">
+        <v>246</v>
+      </c>
+      <c r="D35" t="s">
         <v>247</v>
-      </c>
-      <c r="D35" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -3210,13 +3210,13 @@
         <v>125</v>
       </c>
       <c r="B36" t="s">
+        <v>248</v>
+      </c>
+      <c r="C36" t="s">
         <v>249</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>250</v>
-      </c>
-      <c r="D36" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -3227,10 +3227,10 @@
         <v>179</v>
       </c>
       <c r="C37" t="s">
+        <v>251</v>
+      </c>
+      <c r="D37" t="s">
         <v>252</v>
-      </c>
-      <c r="D37" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -3241,10 +3241,10 @@
         <v>180</v>
       </c>
       <c r="C38" t="s">
+        <v>253</v>
+      </c>
+      <c r="D38" t="s">
         <v>254</v>
-      </c>
-      <c r="D38" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -3252,13 +3252,13 @@
         <v>125</v>
       </c>
       <c r="B39" t="s">
+        <v>255</v>
+      </c>
+      <c r="C39" t="s">
         <v>256</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>257</v>
-      </c>
-      <c r="D39" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -3266,13 +3266,13 @@
         <v>125</v>
       </c>
       <c r="B40" t="s">
+        <v>258</v>
+      </c>
+      <c r="C40" t="s">
         <v>259</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>260</v>
-      </c>
-      <c r="D40" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -3283,10 +3283,10 @@
         <v>157</v>
       </c>
       <c r="C41" t="s">
+        <v>280</v>
+      </c>
+      <c r="D41" t="s">
         <v>281</v>
-      </c>
-      <c r="D41" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -3297,7 +3297,7 @@
         <v>181</v>
       </c>
       <c r="C42" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D42" t="s">
         <v>106</v>
@@ -3311,7 +3311,7 @@
         <v>182</v>
       </c>
       <c r="C43" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D43" t="s">
         <v>107</v>
@@ -3325,10 +3325,10 @@
         <v>183</v>
       </c>
       <c r="C44" t="s">
+        <v>263</v>
+      </c>
+      <c r="D44" t="s">
         <v>264</v>
-      </c>
-      <c r="D44" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -3339,10 +3339,10 @@
         <v>184</v>
       </c>
       <c r="C45" t="s">
+        <v>265</v>
+      </c>
+      <c r="D45" t="s">
         <v>266</v>
-      </c>
-      <c r="D45" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -3353,10 +3353,10 @@
         <v>185</v>
       </c>
       <c r="C46" t="s">
+        <v>267</v>
+      </c>
+      <c r="D46" t="s">
         <v>268</v>
-      </c>
-      <c r="D46" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -3367,7 +3367,7 @@
         <v>186</v>
       </c>
       <c r="C47" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D47" t="s">
         <v>108</v>
@@ -3381,10 +3381,10 @@
         <v>187</v>
       </c>
       <c r="C48" t="s">
+        <v>270</v>
+      </c>
+      <c r="D48" t="s">
         <v>271</v>
-      </c>
-      <c r="D48" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -3395,10 +3395,10 @@
         <v>188</v>
       </c>
       <c r="C49" t="s">
+        <v>272</v>
+      </c>
+      <c r="D49" t="s">
         <v>273</v>
-      </c>
-      <c r="D49" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -3409,7 +3409,7 @@
         <v>189</v>
       </c>
       <c r="C50" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D50" t="s">
         <v>109</v>
@@ -3420,13 +3420,13 @@
         <v>125</v>
       </c>
       <c r="B51" t="s">
+        <v>275</v>
+      </c>
+      <c r="C51" t="s">
         <v>276</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>277</v>
-      </c>
-      <c r="D51" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -3434,13 +3434,13 @@
         <v>125</v>
       </c>
       <c r="B52" t="s">
+        <v>282</v>
+      </c>
+      <c r="C52" t="s">
         <v>283</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>284</v>
-      </c>
-      <c r="D52" t="s">
-        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -3568,7 +3568,7 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B2" t="s">
         <v>89</v>
@@ -3592,7 +3592,7 @@
         <v>93</v>
       </c>
       <c r="K2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -3609,10 +3609,10 @@
         <v>90</v>
       </c>
       <c r="G3" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="H3" s="18" t="s">
         <v>222</v>
-      </c>
-      <c r="H3" s="18" t="s">
-        <v>223</v>
       </c>
       <c r="I3" t="s">
         <v>93</v>
@@ -3667,10 +3667,10 @@
         <v>90</v>
       </c>
       <c r="G5" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="H5" s="18" t="s">
         <v>224</v>
-      </c>
-      <c r="H5" s="18" t="s">
-        <v>225</v>
       </c>
       <c r="I5" t="s">
         <v>93</v>
@@ -3696,10 +3696,10 @@
         <v>90</v>
       </c>
       <c r="G6" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="H6" s="14" t="s">
         <v>226</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>227</v>
       </c>
       <c r="I6" t="s">
         <v>93</v>
@@ -3725,10 +3725,10 @@
         <v>90</v>
       </c>
       <c r="G7" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="H7" s="14" t="s">
         <v>226</v>
-      </c>
-      <c r="H7" s="14" t="s">
-        <v>227</v>
       </c>
       <c r="I7" t="s">
         <v>93</v>
@@ -3751,7 +3751,7 @@
         <v>129</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -3769,7 +3769,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
@@ -3798,10 +3798,10 @@
         <v>110</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>305</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="16.75" customHeight="1">
@@ -3849,24 +3849,24 @@
     </row>
     <row r="7" spans="1:6" s="3" customFormat="1">
       <c r="A7" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F7" s="39" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="3" customFormat="1">
       <c r="A8" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F8" s="39" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -4094,7 +4094,7 @@
         <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="25" spans="1:16384">
@@ -4110,7 +4110,7 @@
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="27" spans="1:16384">
@@ -4150,7 +4150,7 @@
         <v>23</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -20540,7 +20540,7 @@
         <v>28</v>
       </c>
       <c r="B33" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>

</xml_diff>